<commit_message>
Excel 转 Json => ScriptableObject
</commit_message>
<xml_diff>
--- a/Source/Excel/commodity.xlsx
+++ b/Source/Excel/commodity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Game\Source\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Game\Source\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996E7430-386C-41FA-9C6E-E69E80EBA1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF24393F-861E-4E8D-B88E-7980F2F38D47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31785" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,42 +35,64 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>introduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>price</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品2</t>
+  </si>
+  <si>
+    <t>cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品3</t>
+  </si>
+  <si>
+    <t>商品4</t>
+  </si>
+  <si>
+    <t>商品5</t>
+  </si>
+  <si>
+    <t>商品6</t>
+  </si>
+  <si>
+    <t>商品7</t>
+  </si>
+  <si>
+    <t>商品8</t>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>rewards</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[][]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品2</t>
-  </si>
-  <si>
-    <t>cost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase</t>
+    <t>json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -79,6 +101,24 @@
   </si>
   <si>
     <t>[[10001,1],[10002,2]]</t>
+  </si>
+  <si>
+    <t>[[10001,1],[10002,3]]</t>
+  </si>
+  <si>
+    <t>[[10001,1],[10002,4]]</t>
+  </si>
+  <si>
+    <t>[[10001,1],[10002,5]]</t>
+  </si>
+  <si>
+    <t>[[10001,1],[10002,6]]</t>
+  </si>
+  <si>
+    <t>[[10001,1],[10002,7]]</t>
+  </si>
+  <si>
+    <t>[[10001,1],[10002,8]]</t>
   </si>
 </sst>
 </file>
@@ -102,30 +142,37 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <family val="3"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,23 +180,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="60% - 着色 1" xfId="2" builtinId="32"/>
+    <cellStyle name="标题 1" xfId="1" builtinId="16"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,20 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="21.625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="13.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -449,42 +515,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -492,7 +558,7 @@
         <v>1001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>101</v>
@@ -504,10 +570,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -515,7 +581,7 @@
         <v>1002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>102</v>
@@ -527,15 +593,153 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>101</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1004</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>102</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1005</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1006</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
+      <c r="C8" s="1">
+        <v>102</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1007</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1008</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1">
+        <v>102</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>